<commit_message>
changes to TAL, succinic, and HP for FGI paper
</commit_message>
<xml_diff>
--- a/biorefineries/HP/analyses/full/parameter_distributions/acrylic_acid_product/parameter-distributions_sugarcane_Acrylic_300L.xlsx
+++ b/biorefineries/HP/analyses/full/parameter_distributions/acrylic_acid_product/parameter-distributions_sugarcane_Acrylic_300L.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\HP\analyses\full\parameter_distributions\acrylic_acid_product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF0713F-5E38-4E81-9C98-709E88A4472A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865FC969-55F5-462E-BBDD-FE1F804DE5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="980" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>